<commit_message>
Fin du fichier Excel
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73855406b8b524a7/Documents/Openclassroom/Livrable/P5_REUZE_Laurent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25F392F8-2DB3-487B-B870-F81CA4DA4B6B}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C1B40C-699D-4B81-9CAC-C3BA1D66A1CE}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="570" windowWidth="29160" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -130,10 +130,31 @@
     <t>Disparition de l'article de la liste des articles à commander et recalcule des totaux</t>
   </si>
   <si>
-    <t xml:space="preserve">Récupération du contenu du champs email et vérification de </t>
-  </si>
-  <si>
     <t>Affichage de la confirmation de commande</t>
+  </si>
+  <si>
+    <t>Récupération du contenu des différents champs du formulaires, contrôle de la validité du contenu du champs email, envoi de la requete au serveur, récupération du N° de commande  et ouverture de la page confirmation</t>
+  </si>
+  <si>
+    <t>Ouverture de la page confirmation</t>
+  </si>
+  <si>
+    <t>Contrôle du contenu du champs email</t>
+  </si>
+  <si>
+    <t>Récupération du contenu du champs email et vérification de son contenu par le biaix d'un REGEX</t>
+  </si>
+  <si>
+    <t>Affichage d'une alerte si le format de l'adresse email ne correspond pas au format attendu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK / Affichage d'une alerte indiquant : "Le mail saisie ne semble pas être valide. Merci de saisir une adresse mail valide." </t>
+  </si>
+  <si>
+    <t>Récupération du numéro de commande dans l'adresse de la page et affichage du numéro de commande</t>
+  </si>
+  <si>
+    <t>Affichage du numéro de commande</t>
   </si>
 </sst>
 </file>
@@ -683,11 +704,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -817,7 +838,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
@@ -832,7 +855,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
       <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
@@ -847,7 +872,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
       <c r="B10" s="11" t="s">
         <v>26</v>
       </c>
@@ -861,34 +888,56 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
       <c r="B11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="130.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="C13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
@@ -940,11 +989,18 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fin du fichier Powerpoint
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73855406b8b524a7/Documents/Openclassroom/Livrable/P5_REUZE_Laurent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C1B40C-699D-4B81-9CAC-C3BA1D66A1CE}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB1560C6-7DA5-45A9-AE1D-F8F918E1DDCB}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="570" windowWidth="29160" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -161,17 +161,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Montserrat"/>
     </font>
     <font>
       <sz val="14"/>
@@ -179,7 +173,18 @@
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -197,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -371,119 +376,49 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -704,306 +639,243 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="5" customWidth="1"/>
-    <col min="2" max="3" width="58.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="57.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="14.42578125" style="5"/>
+    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:5" ht="93.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+    <row r="4" spans="1:5" ht="93.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="87" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+    <row r="6" spans="1:5" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="87" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+    <row r="7" spans="1:5" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+    <row r="11" spans="1:5" ht="93.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="130.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+    <row r="12" spans="1:5" ht="168.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
+    <row r="13" spans="1:5" ht="93.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>